<commit_message>
modify year option to all forms
</commit_message>
<xml_diff>
--- a/assets/formDoc/GRGP_template.xlsx
+++ b/assets/formDoc/GRGP_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiki\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\gahk-web\assets\formDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A9A1A5-76E6-4A7E-8F8C-C8E60C6DF8E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3503C3-5E3E-45BD-8ED2-635F895C3D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>申請表編號 Application Number</t>
   </si>
@@ -161,13 +161,17 @@
   </si>
   <si>
     <t>隊伍/團體狀況 Team Status</t>
+  </si>
+  <si>
+    <t>比賽年份 Year of Competition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -551,203 +555,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU1"/>
+  <dimension ref="A1:AV1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="30.90625" customWidth="1"/>
-    <col min="2" max="2" width="34.7265625" customWidth="1"/>
-    <col min="3" max="3" width="25.36328125" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" customWidth="1"/>
-    <col min="5" max="5" width="23.54296875" customWidth="1"/>
-    <col min="6" max="6" width="35.81640625" customWidth="1"/>
-    <col min="7" max="7" width="44.1796875" customWidth="1"/>
-    <col min="8" max="8" width="52.453125" customWidth="1"/>
-    <col min="9" max="9" width="45.08984375" customWidth="1"/>
-    <col min="10" max="10" width="44.08984375" customWidth="1"/>
-    <col min="11" max="11" width="46.26953125" customWidth="1"/>
-    <col min="12" max="12" width="42.1796875" customWidth="1"/>
-    <col min="13" max="13" width="53.54296875" customWidth="1"/>
-    <col min="14" max="14" width="43.26953125" customWidth="1"/>
-    <col min="15" max="15" width="42.1796875" customWidth="1"/>
-    <col min="16" max="16" width="46.7265625" customWidth="1"/>
-    <col min="17" max="17" width="40.36328125" customWidth="1"/>
-    <col min="18" max="18" width="52.81640625" customWidth="1"/>
-    <col min="19" max="19" width="42.81640625" customWidth="1"/>
-    <col min="20" max="20" width="42.453125" customWidth="1"/>
-    <col min="21" max="21" width="48.36328125" customWidth="1"/>
-    <col min="22" max="22" width="40.7265625" customWidth="1"/>
-    <col min="23" max="23" width="53.90625" customWidth="1"/>
-    <col min="24" max="24" width="42.1796875" customWidth="1"/>
-    <col min="25" max="25" width="43.08984375" customWidth="1"/>
-    <col min="26" max="26" width="47.08984375" customWidth="1"/>
-    <col min="27" max="27" width="41.81640625" customWidth="1"/>
-    <col min="28" max="28" width="52.6328125" customWidth="1"/>
-    <col min="29" max="29" width="41.81640625" customWidth="1"/>
-    <col min="30" max="30" width="42" customWidth="1"/>
-    <col min="31" max="31" width="46.54296875" customWidth="1"/>
-    <col min="32" max="32" width="40.90625" customWidth="1"/>
-    <col min="33" max="33" width="52.90625" customWidth="1"/>
-    <col min="34" max="34" width="43.7265625" customWidth="1"/>
-    <col min="35" max="35" width="43.08984375" customWidth="1"/>
-    <col min="36" max="36" width="49.54296875" customWidth="1"/>
-    <col min="37" max="37" width="42" customWidth="1"/>
-    <col min="38" max="38" width="31" customWidth="1"/>
-    <col min="39" max="39" width="32.7265625" customWidth="1"/>
-    <col min="40" max="40" width="27" customWidth="1"/>
-    <col min="41" max="41" width="13.26953125" customWidth="1"/>
-    <col min="42" max="42" width="39.453125" customWidth="1"/>
-    <col min="43" max="43" width="16.54296875" customWidth="1"/>
-    <col min="44" max="44" width="19.26953125" customWidth="1"/>
-    <col min="45" max="45" width="23.36328125" customWidth="1"/>
-    <col min="46" max="46" width="20.90625" customWidth="1"/>
-    <col min="47" max="47" width="25.36328125" customWidth="1"/>
+    <col min="1" max="2" width="30.90625" customWidth="1"/>
+    <col min="3" max="3" width="34.7265625" customWidth="1"/>
+    <col min="4" max="4" width="25.36328125" customWidth="1"/>
+    <col min="5" max="5" width="25.81640625" customWidth="1"/>
+    <col min="6" max="6" width="23.54296875" customWidth="1"/>
+    <col min="7" max="7" width="35.81640625" customWidth="1"/>
+    <col min="8" max="8" width="44.1796875" customWidth="1"/>
+    <col min="9" max="9" width="52.453125" customWidth="1"/>
+    <col min="10" max="10" width="45.08984375" customWidth="1"/>
+    <col min="11" max="11" width="44.08984375" customWidth="1"/>
+    <col min="12" max="12" width="46.26953125" customWidth="1"/>
+    <col min="13" max="13" width="42.1796875" customWidth="1"/>
+    <col min="14" max="14" width="53.54296875" customWidth="1"/>
+    <col min="15" max="15" width="43.26953125" customWidth="1"/>
+    <col min="16" max="16" width="42.1796875" customWidth="1"/>
+    <col min="17" max="17" width="46.7265625" customWidth="1"/>
+    <col min="18" max="18" width="40.36328125" customWidth="1"/>
+    <col min="19" max="19" width="52.81640625" customWidth="1"/>
+    <col min="20" max="20" width="42.81640625" customWidth="1"/>
+    <col min="21" max="21" width="42.453125" customWidth="1"/>
+    <col min="22" max="22" width="48.36328125" customWidth="1"/>
+    <col min="23" max="23" width="40.7265625" customWidth="1"/>
+    <col min="24" max="24" width="53.90625" customWidth="1"/>
+    <col min="25" max="25" width="42.1796875" customWidth="1"/>
+    <col min="26" max="26" width="43.08984375" customWidth="1"/>
+    <col min="27" max="27" width="47.08984375" customWidth="1"/>
+    <col min="28" max="28" width="41.81640625" customWidth="1"/>
+    <col min="29" max="29" width="52.6328125" customWidth="1"/>
+    <col min="30" max="30" width="41.81640625" customWidth="1"/>
+    <col min="31" max="31" width="42" customWidth="1"/>
+    <col min="32" max="32" width="46.54296875" customWidth="1"/>
+    <col min="33" max="33" width="40.90625" customWidth="1"/>
+    <col min="34" max="34" width="52.90625" customWidth="1"/>
+    <col min="35" max="35" width="43.7265625" customWidth="1"/>
+    <col min="36" max="36" width="43.08984375" customWidth="1"/>
+    <col min="37" max="37" width="49.54296875" customWidth="1"/>
+    <col min="38" max="38" width="42" customWidth="1"/>
+    <col min="39" max="39" width="31" customWidth="1"/>
+    <col min="40" max="40" width="32.7265625" customWidth="1"/>
+    <col min="41" max="41" width="27" customWidth="1"/>
+    <col min="42" max="42" width="13.26953125" customWidth="1"/>
+    <col min="43" max="43" width="39.453125" customWidth="1"/>
+    <col min="44" max="44" width="16.54296875" customWidth="1"/>
+    <col min="45" max="45" width="19.26953125" customWidth="1"/>
+    <col min="46" max="46" width="23.36328125" customWidth="1"/>
+    <col min="47" max="47" width="20.90625" customWidth="1"/>
+    <col min="48" max="48" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -756,7 +763,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:AU1" numberStoredAsText="1"/>
+    <ignoredError sqref="C1:AV1 A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>